<commit_message>
Modify scheme: statue_height => partial_height
</commit_message>
<xml_diff>
--- a/jizo_project.xlsx
+++ b/jizo_project.xlsx
@@ -442,7 +442,7 @@
         <v>総高</v>
       </c>
       <c r="T1" t="str">
-        <v>像高</v>
+        <v>部分高</v>
       </c>
       <c r="U1" t="str">
         <v>幅</v>
@@ -10193,7 +10193,7 @@
         <v>西御門町</v>
       </c>
       <c r="L237" t="str" xml:space="preserve">
-        <v xml:space="preserve">元要記によると、神亀2年（725年）7月22日に平城七御門が整備され、それぞれに北斗七星の七星が祀られた時に、西御門町には文曲星と豊斟渟尊（とよくむぬのみこと）を祀って桑の木が植えられたとされています。その文曲星の社が途切れず存続したのか廃亡再興を繰り返したのかはわかりませんが、寛政年間（1800年頃）に記された平城坊目考には、現在（書かれた時代から見ての現在なので江戸時代です）三座の神を祀った小社とその北側に会所があるところがその文曲星の社の遺跡だと伝わっていたと書かれており、その時の祭神は左が春日神、中が文曲星、右が住吉神だったそうです。当時の町の古老が言うには、春日大社が御笠山に鎮座した神護景雲2年（768年）、空に瑞雲がたったのを初めて目撃した（見初めた）場所がここだったので、今も見初（みそめ）神社と呼ぶということだったようです。伝説とはいえ、実に40年以上春日大社より古い由緒を持つ神社という事で驚きです。会所には観音堂が付属していたと、また別の地誌である奈良坊目拙解（享保15年、1730年成立とされる）には記録されています。_x000d_
+        <v xml:space="preserve">元要記によると、神亀2年（725年）7月22日に平城七御門が整備され、それぞれに北斗七星の七星が祀られた時に、西御門町には文曲星と豊斟渟尊（とよくむぬのみこと）を祀って桑の木が植えられたとされています。その文曲星の社が途切れず存続したのか廃亡再興を繰り返したのかはわかりませんが、寛政年間（1800年頃）に記された平城坊目考には、現在（書かれた時代から見ての現在なので江戸時代です）三座の神を祀った小社とその北側に会所があるところがその文曲星の社の遺跡だと伝わっていたと書かれており、その時の祭神は左が春日神、中が文曲星、右が住吉神だったそうです。当時の町の古老が言うには、春日大社が御笠山に鎮座した神護景雲2年（768年）、空に瑞雲がたったのを初めて目撃した（見初めた）場所がここだったので、今も見初（みそめ）神社と呼ぶということだったようです。伝説とはいえ、実に40年以上春日大社より古い由緒を持つ神社という事で驚きです。会所には観音堂が付属していたと、また別の地誌である奈良坊目拙解（享保15年、1730年成立とされる）には記録されています。_x000d__x000d_
 現在の祭神は、奈良市史社寺編によると、天忍雲根命（あめのおしくもねのみこと）、底筒男神（そこつつのおのかみ）、金山彦神（かなやまひこのかみ）の三座ということです。天忍雲根命は春日若宮、底筒男神は住吉三神の一柱ですから、文曲星は金山彦神に変わったのでしょうか。北には会所もあり、木造観世音菩薩や地蔵立像が安置されているそうで、江戸期の観音堂の名残でしょうか。北西には石地蔵が祀られた地蔵堂もあります。</v>
       </c>
       <c r="O237" t="str">
@@ -22506,8 +22506,8 @@
         <v>歌姫町</v>
       </c>
       <c r="O534" t="str" xml:space="preserve">
-        <v xml:space="preserve">歌姫町 六大地蔵尊_x000d_
-地元の90歳のお婆さんに、「ろくたいじぞう」様だと教えてもらいました 「たい」が「体」か「大」かはよくわかりません_x000d_
+        <v xml:space="preserve">歌姫町 六大地蔵尊_x000d__x000d_
+地元の90歳のお婆さんに、「ろくたいじぞう」様だと教えてもらいました 「たい」が「体」か「大」かはよくわかりません_x000d__x000d_
 また、道の向こうとこちらで佐紀町と歌姫町が分かれるうち、佐紀町側の守り地蔵だと伺った気がしますが、地図によると墓地は歌姫町に属するので、それもよくわかりません</v>
       </c>
       <c r="P534" t="str">

</xml_diff>

<commit_message>
Add the survey results of Mr. Onoue and Mr. Hidaka
</commit_message>
<xml_diff>
--- a/jizo_project.xlsx
+++ b/jizo_project.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE576"/>
+  <dimension ref="A1:AE585"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1046,7 +1046,7 @@
         <v>東向北町</v>
       </c>
       <c r="P13" t="str">
-        <v>2022-07-23</v>
+        <v>2023-07-23</v>
       </c>
       <c r="Q13" t="b">
         <v>1</v>
@@ -2588,7 +2588,7 @@
         <v>地蔵</v>
       </c>
       <c r="C46" t="str">
-        <v>地蔵堂</v>
+        <v>橋北地蔵尊</v>
       </c>
       <c r="F46" t="str">
         <v>奈良県</v>
@@ -2606,7 +2606,7 @@
         <v>川上町 丘の中腹</v>
       </c>
       <c r="P46" t="str">
-        <v>2022-07-23</v>
+        <v>2023-07-23</v>
       </c>
       <c r="Q46" t="b">
         <v>1</v>
@@ -3226,7 +3226,7 @@
         <v>手貝町 転害門脇</v>
       </c>
       <c r="P59" t="str">
-        <v>2016-11-04</v>
+        <v>2023-07-23</v>
       </c>
       <c r="Q59" t="b">
         <v>1</v>
@@ -3236,6 +3236,9 @@
       </c>
       <c r="W59" t="str">
         <v/>
+      </c>
+      <c r="X59" t="str">
+        <v>石造</v>
       </c>
       <c r="AC59" t="str">
         <v/>
@@ -4360,7 +4363,7 @@
         <v>花芝町</v>
       </c>
       <c r="P83" t="str">
-        <v>2022-07-23</v>
+        <v>2023-07-23</v>
       </c>
       <c r="Q83" t="b">
         <v>1</v>
@@ -6293,7 +6296,7 @@
         <v>川上町</v>
       </c>
       <c r="P124" t="str">
-        <v>2022-07-23</v>
+        <v>2023-07-23</v>
       </c>
       <c r="Q124" t="b">
         <v>1</v>
@@ -7242,7 +7245,7 @@
         <v>興善院町</v>
       </c>
       <c r="P144" t="str">
-        <v>2016-02-19</v>
+        <v>2023-07-23</v>
       </c>
       <c r="Q144" t="b">
         <v>1</v>
@@ -20747,7 +20750,7 @@
         <v>法蓮町 浮彫五輪塔群</v>
       </c>
       <c r="P428" t="str">
-        <v>2017-05-03</v>
+        <v>2023-07-23</v>
       </c>
       <c r="Q428" t="b">
         <v>1</v>
@@ -26381,7 +26384,7 @@
         <v>法蓮町</v>
       </c>
       <c r="P547" t="str">
-        <v>2022-10-01</v>
+        <v>2023-07-23</v>
       </c>
       <c r="Q547" t="b">
         <v>1</v>
@@ -27803,16 +27806,442 @@
         <v>34.715620055120674</v>
       </c>
     </row>
+    <row r="577">
+      <c r="A577">
+        <v>852</v>
+      </c>
+      <c r="B577" t="str">
+        <v>地蔵</v>
+      </c>
+      <c r="C577" t="str">
+        <v>恋ノ窪地蔵尊（吉原地蔵尊）</v>
+      </c>
+      <c r="D577" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F577" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G577" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H577" t="str">
+        <v>大安寺</v>
+      </c>
+      <c r="I577" t="str">
+        <v>恋の窪２丁目</v>
+      </c>
+      <c r="O577" t="str">
+        <v>恋ノ窪地蔵尊（吉原地蔵尊）</v>
+      </c>
+      <c r="P577" t="str">
+        <v>2023-08-02</v>
+      </c>
+      <c r="Q577" t="b">
+        <v>1</v>
+      </c>
+      <c r="R577">
+        <v>1753</v>
+      </c>
+      <c r="X577" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD577">
+        <v>135.80825020325707</v>
+      </c>
+      <c r="AE577">
+        <v>34.67419542400422</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578">
+        <v>853</v>
+      </c>
+      <c r="B578" t="str">
+        <v>地蔵</v>
+      </c>
+      <c r="C578" t="str">
+        <v>大日地蔵菩薩</v>
+      </c>
+      <c r="D578" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F578" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G578" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H578" t="str">
+        <v>佐保</v>
+      </c>
+      <c r="I578" t="str">
+        <v>法蓮町</v>
+      </c>
+      <c r="L578" t="str">
+        <v/>
+      </c>
+      <c r="O578" t="str">
+        <v>大日地蔵菩薩</v>
+      </c>
+      <c r="P578" t="str">
+        <v>2023-08-02</v>
+      </c>
+      <c r="Q578" t="b">
+        <v>1</v>
+      </c>
+      <c r="R578">
+        <v>1757</v>
+      </c>
+      <c r="X578" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD578">
+        <v>135.8178877018412</v>
+      </c>
+      <c r="AE578">
+        <v>34.69398748871348</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579">
+        <v>854</v>
+      </c>
+      <c r="B579" t="str">
+        <v>地蔵</v>
+      </c>
+      <c r="C579" t="str">
+        <v>法華寺町地蔵堂</v>
+      </c>
+      <c r="D579" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F579" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G579" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H579" t="str">
+        <v>佐保</v>
+      </c>
+      <c r="I579" t="str">
+        <v>法華寺町</v>
+      </c>
+      <c r="O579" t="str">
+        <v>法華寺町地蔵堂</v>
+      </c>
+      <c r="P579" t="str">
+        <v>2023-08-02</v>
+      </c>
+      <c r="Q579" t="b">
+        <v>1</v>
+      </c>
+      <c r="R579">
+        <v>1762</v>
+      </c>
+      <c r="X579" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD579">
+        <v>135.81137160953628</v>
+      </c>
+      <c r="AE579">
+        <v>34.69694759352076</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580">
+        <v>855</v>
+      </c>
+      <c r="B580" t="str">
+        <v>地蔵</v>
+      </c>
+      <c r="C580" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="D580" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F580" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G580" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H580" t="str">
+        <v>佐保</v>
+      </c>
+      <c r="I580" t="str">
+        <v>法蓮町</v>
+      </c>
+      <c r="O580" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="P580" t="str">
+        <v>2023-08-02</v>
+      </c>
+      <c r="Q580" t="b">
+        <v>1</v>
+      </c>
+      <c r="R580">
+        <v>1766</v>
+      </c>
+      <c r="X580" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD580">
+        <v>135.8131608815159</v>
+      </c>
+      <c r="AE580">
+        <v>34.69588772600773</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581">
+        <v>856</v>
+      </c>
+      <c r="B581" t="str">
+        <v>地蔵</v>
+      </c>
+      <c r="C581" t="str">
+        <v>川上町掘り起こし地蔵</v>
+      </c>
+      <c r="D581" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F581" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G581" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H581" t="str">
+        <v>鼓阪</v>
+      </c>
+      <c r="I581" t="str">
+        <v>川上町</v>
+      </c>
+      <c r="O581" t="str">
+        <v>川上町の住宅造成で掘り起こされた地蔵</v>
+      </c>
+      <c r="P581" t="str">
+        <v>2023-07-23</v>
+      </c>
+      <c r="Q581" t="b">
+        <v>1</v>
+      </c>
+      <c r="R581">
+        <v>1773</v>
+      </c>
+      <c r="X581" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD581">
+        <v>135.83244423586274</v>
+      </c>
+      <c r="AE581">
+        <v>34.69376795026089</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582">
+        <v>857</v>
+      </c>
+      <c r="B582" t="str">
+        <v>五輪塔</v>
+      </c>
+      <c r="C582" t="str">
+        <v>持宝院五輪塔、浮彫五輪塔</v>
+      </c>
+      <c r="D582" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F582" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G582" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H582" t="str">
+        <v>鼓阪</v>
+      </c>
+      <c r="I582" t="str">
+        <v>雑司町</v>
+      </c>
+      <c r="O582" t="str">
+        <v>持宝院の五輪塔、浮彫五輪塔</v>
+      </c>
+      <c r="P582" t="str">
+        <v>2023-07-23</v>
+      </c>
+      <c r="Q582" t="b">
+        <v>1</v>
+      </c>
+      <c r="R582">
+        <v>1780</v>
+      </c>
+      <c r="X582" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD582">
+        <v>135.84185441918297</v>
+      </c>
+      <c r="AE582">
+        <v>34.690904105412685</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583">
+        <v>858</v>
+      </c>
+      <c r="B583" t="str">
+        <v>地蔵</v>
+      </c>
+      <c r="C583" t="str">
+        <v>正倉院東方地蔵群</v>
+      </c>
+      <c r="D583" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F583" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G583" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H583" t="str">
+        <v>鼓阪</v>
+      </c>
+      <c r="I583" t="str">
+        <v>雑司町</v>
+      </c>
+      <c r="O583" t="str">
+        <v>正倉院東方の地蔵群</v>
+      </c>
+      <c r="P583" t="str">
+        <v>2023-07-23</v>
+      </c>
+      <c r="Q583" t="b">
+        <v>1</v>
+      </c>
+      <c r="R583">
+        <v>1781</v>
+      </c>
+      <c r="X583" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD583">
+        <v>135.83979521032842</v>
+      </c>
+      <c r="AE583">
+        <v>34.69097419529438</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584">
+        <v>859</v>
+      </c>
+      <c r="B584" t="str">
+        <v>地蔵</v>
+      </c>
+      <c r="C584" t="str">
+        <v>西大寺赤田町地蔵堂１</v>
+      </c>
+      <c r="D584" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F584" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G584" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H584" t="str">
+        <v>伏見</v>
+      </c>
+      <c r="I584" t="str">
+        <v>西大寺赤田町１丁目</v>
+      </c>
+      <c r="O584" t="str">
+        <v>西大寺赤田町地蔵堂１</v>
+      </c>
+      <c r="P584" t="str">
+        <v>2023-05-10</v>
+      </c>
+      <c r="Q584" t="b">
+        <v>1</v>
+      </c>
+      <c r="R584">
+        <v>1786</v>
+      </c>
+      <c r="X584" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD584">
+        <v>135.77458414421153</v>
+      </c>
+      <c r="AE584">
+        <v>34.698455605276955</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585">
+        <v>860</v>
+      </c>
+      <c r="B585" t="str">
+        <v>地蔵</v>
+      </c>
+      <c r="C585" t="str">
+        <v>西大寺赤田町地蔵堂２</v>
+      </c>
+      <c r="D585" t="str">
+        <v>不明</v>
+      </c>
+      <c r="F585" t="str">
+        <v>奈良県</v>
+      </c>
+      <c r="G585" t="str">
+        <v>奈良市</v>
+      </c>
+      <c r="H585" t="str">
+        <v>伏見</v>
+      </c>
+      <c r="I585" t="str">
+        <v>西大寺赤田町１丁目</v>
+      </c>
+      <c r="O585" t="str">
+        <v>西大寺赤田町地蔵堂２</v>
+      </c>
+      <c r="P585" t="str">
+        <v>2023-05-10</v>
+      </c>
+      <c r="Q585" t="b">
+        <v>1</v>
+      </c>
+      <c r="R585">
+        <v>1788</v>
+      </c>
+      <c r="X585" t="str">
+        <v>石造</v>
+      </c>
+      <c r="AD585">
+        <v>135.77456575841816</v>
+      </c>
+      <c r="AE585">
+        <v>34.69844736015697</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE576"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE585"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1744"/>
+  <dimension ref="A1:H1784"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -31361,7 +31790,7 @@
         <v>45</v>
       </c>
       <c r="C137" t="str">
-        <v>川上町 地蔵堂（丘の中腹）遠景</v>
+        <v>橋北地蔵尊遠景</v>
       </c>
       <c r="D137" t="str">
         <v>./images/45/Jizodo_(Kawakamicho,_Hill_Side)_Nara_From_Far.jpg</v>
@@ -31387,7 +31816,7 @@
         <v>45</v>
       </c>
       <c r="C138" t="str">
-        <v>川上町 地蔵堂（丘の中腹）内部</v>
+        <v>橋北地蔵尊内部</v>
       </c>
       <c r="D138" t="str">
         <v>./images/45/Jizodo_(Kawakamicho,_Hill_Side)_Nara_Inside_1.jpg</v>
@@ -31413,7 +31842,7 @@
         <v>45</v>
       </c>
       <c r="C139" t="str">
-        <v>川上町 地蔵堂（丘の中腹）内部</v>
+        <v>橋北地蔵尊内部</v>
       </c>
       <c r="D139" t="str">
         <v>./images/45/Jizodo_(Kawakamicho,_Hill_Side)_Nara_Inside_2.jpg</v>
@@ -31439,7 +31868,7 @@
         <v>45</v>
       </c>
       <c r="C140" t="str">
-        <v>川上町 地蔵堂（丘の中腹）</v>
+        <v>橋北地蔵尊</v>
       </c>
       <c r="D140" t="str">
         <v>./images/45/Jizodo_(Kawakamicho,_Hill_Side)_Nara.jpg</v>
@@ -69633,7 +70062,7 @@
         <v>45</v>
       </c>
       <c r="C1609" t="str">
-        <v>川上町 丘の中腹 地蔵堂 令和4年地蔵盆 内部</v>
+        <v>橋北地蔵尊 令和4年地蔵盆 内部</v>
       </c>
       <c r="D1609" t="str">
         <v>./images/45/IMG_9188.jpg</v>
@@ -69659,7 +70088,7 @@
         <v>45</v>
       </c>
       <c r="C1610" t="str">
-        <v>川上町 丘の中腹 地蔵堂 令和4年地蔵盆</v>
+        <v>橋北地蔵尊 令和4年地蔵盆</v>
       </c>
       <c r="D1610" t="str">
         <v>./images/45/IMG_9189.jpg</v>
@@ -73161,9 +73590,1049 @@
         <v>./small_thumbs/851/327036517_1212205186347542_1456052015830501280_n.jpg</v>
       </c>
     </row>
+    <row r="1745">
+      <c r="A1745">
+        <v>1751</v>
+      </c>
+      <c r="B1745">
+        <v>75</v>
+      </c>
+      <c r="C1745" t="str">
+        <v>地蔵堂</v>
+      </c>
+      <c r="D1745" t="str">
+        <v>./images/75/61934.jpg</v>
+      </c>
+      <c r="E1745" t="str">
+        <v>2023-07-26T00:00:00</v>
+      </c>
+      <c r="F1745" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1745" t="str">
+        <v>./mid_thumbs/75/61934.jpg</v>
+      </c>
+      <c r="H1745" t="str">
+        <v>./small_thumbs/75/61934.jpg</v>
+      </c>
+    </row>
+    <row r="1746">
+      <c r="A1746">
+        <v>1752</v>
+      </c>
+      <c r="B1746">
+        <v>75</v>
+      </c>
+      <c r="C1746" t="str">
+        <v>地蔵堂</v>
+      </c>
+      <c r="D1746" t="str">
+        <v>./images/75/61935.jpg</v>
+      </c>
+      <c r="E1746" t="str">
+        <v>2023-07-26T00:00:00</v>
+      </c>
+      <c r="F1746" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1746" t="str">
+        <v>./mid_thumbs/75/61935.jpg</v>
+      </c>
+      <c r="H1746" t="str">
+        <v>./small_thumbs/75/61935.jpg</v>
+      </c>
+    </row>
+    <row r="1747">
+      <c r="A1747">
+        <v>1753</v>
+      </c>
+      <c r="B1747">
+        <v>852</v>
+      </c>
+      <c r="C1747" t="str">
+        <v>恋ノ窪地蔵尊（吉原地蔵尊）</v>
+      </c>
+      <c r="D1747" t="str">
+        <v>./images/852/61927.jpg</v>
+      </c>
+      <c r="E1747" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1747" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1747" t="str">
+        <v>./mid_thumbs/852/61927.jpg</v>
+      </c>
+      <c r="H1747" t="str">
+        <v>./small_thumbs/852/61927.jpg</v>
+      </c>
+    </row>
+    <row r="1748">
+      <c r="A1748">
+        <v>1754</v>
+      </c>
+      <c r="B1748">
+        <v>852</v>
+      </c>
+      <c r="C1748" t="str">
+        <v>恋ノ窪地蔵尊（吉原地蔵尊）</v>
+      </c>
+      <c r="D1748" t="str">
+        <v>./images/852/61928.jpg</v>
+      </c>
+      <c r="E1748" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1748" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1748" t="str">
+        <v>./mid_thumbs/852/61928.jpg</v>
+      </c>
+      <c r="H1748" t="str">
+        <v>./small_thumbs/852/61928.jpg</v>
+      </c>
+    </row>
+    <row r="1749">
+      <c r="A1749">
+        <v>1755</v>
+      </c>
+      <c r="B1749">
+        <v>852</v>
+      </c>
+      <c r="C1749" t="str">
+        <v>恋ノ窪地蔵尊（吉原地蔵尊）</v>
+      </c>
+      <c r="D1749" t="str">
+        <v>./images/852/61929.jpg</v>
+      </c>
+      <c r="E1749" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1749" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1749" t="str">
+        <v>./mid_thumbs/852/61929.jpg</v>
+      </c>
+      <c r="H1749" t="str">
+        <v>./small_thumbs/852/61929.jpg</v>
+      </c>
+    </row>
+    <row r="1750">
+      <c r="A1750">
+        <v>1756</v>
+      </c>
+      <c r="B1750">
+        <v>853</v>
+      </c>
+      <c r="C1750" t="str">
+        <v>大日地蔵菩薩 地蔵堂内部</v>
+      </c>
+      <c r="D1750" t="str">
+        <v>./images/853/IMG_8030.jpg</v>
+      </c>
+      <c r="E1750" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1750" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1750" t="str">
+        <v>./mid_thumbs/853/IMG_8030.jpg</v>
+      </c>
+      <c r="H1750" t="str">
+        <v>./small_thumbs/853/IMG_8030.jpg</v>
+      </c>
+    </row>
+    <row r="1751">
+      <c r="A1751">
+        <v>1757</v>
+      </c>
+      <c r="B1751">
+        <v>853</v>
+      </c>
+      <c r="C1751" t="str">
+        <v>大日地蔵菩薩 地蔵堂</v>
+      </c>
+      <c r="D1751" t="str">
+        <v>./images/853/IMG_8031.jpg</v>
+      </c>
+      <c r="E1751" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1751" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1751" t="str">
+        <v>./mid_thumbs/853/IMG_8031.jpg</v>
+      </c>
+      <c r="H1751" t="str">
+        <v>./small_thumbs/853/IMG_8031.jpg</v>
+      </c>
+    </row>
+    <row r="1752">
+      <c r="A1752">
+        <v>1758</v>
+      </c>
+      <c r="B1752">
+        <v>853</v>
+      </c>
+      <c r="C1752" t="str">
+        <v>大日地蔵菩薩 地蔵堂</v>
+      </c>
+      <c r="D1752" t="str">
+        <v>./images/853/IMG_8032.jpg</v>
+      </c>
+      <c r="E1752" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1752" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1752" t="str">
+        <v>./mid_thumbs/853/IMG_8032.jpg</v>
+      </c>
+      <c r="H1752" t="str">
+        <v>./small_thumbs/853/IMG_8032.jpg</v>
+      </c>
+    </row>
+    <row r="1753">
+      <c r="A1753">
+        <v>1759</v>
+      </c>
+      <c r="B1753">
+        <v>853</v>
+      </c>
+      <c r="C1753" t="str">
+        <v>大日地蔵菩薩 扁額</v>
+      </c>
+      <c r="D1753" t="str">
+        <v>./images/853/IMG_8033.jpg</v>
+      </c>
+      <c r="E1753" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1753" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1753" t="str">
+        <v>./mid_thumbs/853/IMG_8033.jpg</v>
+      </c>
+      <c r="H1753" t="str">
+        <v>./small_thumbs/853/IMG_8033.jpg</v>
+      </c>
+    </row>
+    <row r="1754">
+      <c r="A1754">
+        <v>1760</v>
+      </c>
+      <c r="B1754">
+        <v>853</v>
+      </c>
+      <c r="C1754" t="str">
+        <v>大日地蔵菩薩 地蔵堂</v>
+      </c>
+      <c r="D1754" t="str">
+        <v>./images/853/IMG_8034.jpg</v>
+      </c>
+      <c r="E1754" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1754" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1754" t="str">
+        <v>./mid_thumbs/853/IMG_8034.jpg</v>
+      </c>
+      <c r="H1754" t="str">
+        <v>./small_thumbs/853/IMG_8034.jpg</v>
+      </c>
+    </row>
+    <row r="1755">
+      <c r="A1755">
+        <v>1761</v>
+      </c>
+      <c r="B1755">
+        <v>854</v>
+      </c>
+      <c r="C1755" t="str">
+        <v>法華寺町地蔵堂</v>
+      </c>
+      <c r="D1755" t="str">
+        <v>./images/854/IMG_8036.jpg</v>
+      </c>
+      <c r="E1755" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1755" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1755" t="str">
+        <v>./mid_thumbs/854/IMG_8036.jpg</v>
+      </c>
+      <c r="H1755" t="str">
+        <v>./small_thumbs/854/IMG_8036.jpg</v>
+      </c>
+    </row>
+    <row r="1756">
+      <c r="A1756">
+        <v>1762</v>
+      </c>
+      <c r="B1756">
+        <v>854</v>
+      </c>
+      <c r="C1756" t="str">
+        <v>法華寺町地蔵堂</v>
+      </c>
+      <c r="D1756" t="str">
+        <v>./images/854/IMG_8037.jpg</v>
+      </c>
+      <c r="E1756" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1756" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1756" t="str">
+        <v>./mid_thumbs/854/IMG_8037.jpg</v>
+      </c>
+      <c r="H1756" t="str">
+        <v>./small_thumbs/854/IMG_8037.jpg</v>
+      </c>
+    </row>
+    <row r="1757">
+      <c r="A1757">
+        <v>1763</v>
+      </c>
+      <c r="B1757">
+        <v>855</v>
+      </c>
+      <c r="C1757" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="D1757" t="str">
+        <v>./images/855/IMG_8039.jpg</v>
+      </c>
+      <c r="E1757" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1757" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1757" t="str">
+        <v>./mid_thumbs/855/IMG_8039.jpg</v>
+      </c>
+      <c r="H1757" t="str">
+        <v>./small_thumbs/855/IMG_8039.jpg</v>
+      </c>
+    </row>
+    <row r="1758">
+      <c r="A1758">
+        <v>1764</v>
+      </c>
+      <c r="B1758">
+        <v>855</v>
+      </c>
+      <c r="C1758" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="D1758" t="str">
+        <v>./images/855/IMG_8040.jpg</v>
+      </c>
+      <c r="E1758" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1758" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1758" t="str">
+        <v>./mid_thumbs/855/IMG_8040.jpg</v>
+      </c>
+      <c r="H1758" t="str">
+        <v>./small_thumbs/855/IMG_8040.jpg</v>
+      </c>
+    </row>
+    <row r="1759">
+      <c r="A1759">
+        <v>1765</v>
+      </c>
+      <c r="B1759">
+        <v>855</v>
+      </c>
+      <c r="C1759" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="D1759" t="str">
+        <v>./images/855/IMG_8041.jpg</v>
+      </c>
+      <c r="E1759" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1759" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1759" t="str">
+        <v>./mid_thumbs/855/IMG_8041.jpg</v>
+      </c>
+      <c r="H1759" t="str">
+        <v>./small_thumbs/855/IMG_8041.jpg</v>
+      </c>
+    </row>
+    <row r="1760">
+      <c r="A1760">
+        <v>1766</v>
+      </c>
+      <c r="B1760">
+        <v>855</v>
+      </c>
+      <c r="C1760" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="D1760" t="str">
+        <v>./images/855/IMG_8042.jpg</v>
+      </c>
+      <c r="E1760" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1760" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1760" t="str">
+        <v>./mid_thumbs/855/IMG_8042.jpg</v>
+      </c>
+      <c r="H1760" t="str">
+        <v>./small_thumbs/855/IMG_8042.jpg</v>
+      </c>
+    </row>
+    <row r="1761">
+      <c r="A1761">
+        <v>1767</v>
+      </c>
+      <c r="B1761">
+        <v>855</v>
+      </c>
+      <c r="C1761" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="D1761" t="str">
+        <v>./images/855/IMG_8043.jpg</v>
+      </c>
+      <c r="E1761" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1761" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1761" t="str">
+        <v>./mid_thumbs/855/IMG_8043.jpg</v>
+      </c>
+      <c r="H1761" t="str">
+        <v>./small_thumbs/855/IMG_8043.jpg</v>
+      </c>
+    </row>
+    <row r="1762">
+      <c r="A1762">
+        <v>1768</v>
+      </c>
+      <c r="B1762">
+        <v>855</v>
+      </c>
+      <c r="C1762" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="D1762" t="str">
+        <v>./images/855/IMG_8044.jpg</v>
+      </c>
+      <c r="E1762" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1762" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1762" t="str">
+        <v>./mid_thumbs/855/IMG_8044.jpg</v>
+      </c>
+      <c r="H1762" t="str">
+        <v>./small_thumbs/855/IMG_8044.jpg</v>
+      </c>
+    </row>
+    <row r="1763">
+      <c r="A1763">
+        <v>1769</v>
+      </c>
+      <c r="B1763">
+        <v>855</v>
+      </c>
+      <c r="C1763" t="str">
+        <v>佐保田念仏講墓地地蔵群</v>
+      </c>
+      <c r="D1763" t="str">
+        <v>./images/855/IMG_8045.jpg</v>
+      </c>
+      <c r="E1763" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1763" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1763" t="str">
+        <v>./mid_thumbs/855/IMG_8045.jpg</v>
+      </c>
+      <c r="H1763" t="str">
+        <v>./small_thumbs/855/IMG_8045.jpg</v>
+      </c>
+    </row>
+    <row r="1764">
+      <c r="A1764">
+        <v>1770</v>
+      </c>
+      <c r="B1764">
+        <v>701</v>
+      </c>
+      <c r="C1764" t="str">
+        <v>浮彫五輪塔群</v>
+      </c>
+      <c r="D1764" t="str">
+        <v>./images/701/IMG_8047.jpg</v>
+      </c>
+      <c r="E1764" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1764" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1764" t="str">
+        <v>./mid_thumbs/701/IMG_8047.jpg</v>
+      </c>
+      <c r="H1764" t="str">
+        <v>./small_thumbs/701/IMG_8047.jpg</v>
+      </c>
+    </row>
+    <row r="1765">
+      <c r="A1765">
+        <v>1771</v>
+      </c>
+      <c r="B1765">
+        <v>701</v>
+      </c>
+      <c r="C1765" t="str">
+        <v>浮彫五輪塔群</v>
+      </c>
+      <c r="D1765" t="str">
+        <v>./images/701/IMG_8048.jpg</v>
+      </c>
+      <c r="E1765" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1765" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1765" t="str">
+        <v>./mid_thumbs/701/IMG_8048.jpg</v>
+      </c>
+      <c r="H1765" t="str">
+        <v>./small_thumbs/701/IMG_8048.jpg</v>
+      </c>
+    </row>
+    <row r="1766">
+      <c r="A1766">
+        <v>1772</v>
+      </c>
+      <c r="B1766">
+        <v>822</v>
+      </c>
+      <c r="C1766" t="str">
+        <v>法蓮不退寺野神脇の地蔵群</v>
+      </c>
+      <c r="D1766" t="str">
+        <v>./images/822/IMG_8050.jpg</v>
+      </c>
+      <c r="E1766" t="str">
+        <v>2023-08-02T00:00:00</v>
+      </c>
+      <c r="F1766" t="str">
+        <v>J.Onoue</v>
+      </c>
+      <c r="G1766" t="str">
+        <v>./mid_thumbs/822/IMG_8050.jpg</v>
+      </c>
+      <c r="H1766" t="str">
+        <v>./small_thumbs/822/IMG_8050.jpg</v>
+      </c>
+    </row>
+    <row r="1767">
+      <c r="A1767">
+        <v>1773</v>
+      </c>
+      <c r="B1767">
+        <v>856</v>
+      </c>
+      <c r="C1767" t="str">
+        <v>川上町掘り起こし地蔵</v>
+      </c>
+      <c r="D1767" t="str">
+        <v>./images/856/IMG_7943.jpg</v>
+      </c>
+      <c r="E1767" t="str">
+        <v>2023-07-23T14:52:41</v>
+      </c>
+      <c r="F1767" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1767" t="str">
+        <v>./mid_thumbs/856/IMG_7943.jpg</v>
+      </c>
+      <c r="H1767" t="str">
+        <v>./small_thumbs/856/IMG_7943.jpg</v>
+      </c>
+    </row>
+    <row r="1768">
+      <c r="A1768">
+        <v>1774</v>
+      </c>
+      <c r="B1768">
+        <v>856</v>
+      </c>
+      <c r="C1768" t="str">
+        <v>川上町掘り起こし地蔵</v>
+      </c>
+      <c r="D1768" t="str">
+        <v>./images/856/IMG_7944.jpg</v>
+      </c>
+      <c r="E1768" t="str">
+        <v>2023-07-23T14:52:47</v>
+      </c>
+      <c r="F1768" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1768" t="str">
+        <v>./mid_thumbs/856/IMG_7944.jpg</v>
+      </c>
+      <c r="H1768" t="str">
+        <v>./small_thumbs/856/IMG_7944.jpg</v>
+      </c>
+    </row>
+    <row r="1769">
+      <c r="A1769">
+        <v>1775</v>
+      </c>
+      <c r="B1769">
+        <v>143</v>
+      </c>
+      <c r="C1769" t="str">
+        <v>夕日地蔵 地蔵盆</v>
+      </c>
+      <c r="D1769" t="str">
+        <v>./images/143/IMG_7938.jpg</v>
+      </c>
+      <c r="E1769" t="str">
+        <v>2023-07-23T14:27:06</v>
+      </c>
+      <c r="F1769" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1769" t="str">
+        <v>./mid_thumbs/143/IMG_7938.jpg</v>
+      </c>
+      <c r="H1769" t="str">
+        <v>./small_thumbs/143/IMG_7938.jpg</v>
+      </c>
+    </row>
+    <row r="1770">
+      <c r="A1770">
+        <v>1776</v>
+      </c>
+      <c r="B1770">
+        <v>123</v>
+      </c>
+      <c r="C1770" t="str">
+        <v>佐保川地蔵尊 地蔵盆</v>
+      </c>
+      <c r="D1770" t="str">
+        <v>./images/123/IMG_7939.jpg</v>
+      </c>
+      <c r="E1770" t="str">
+        <v>2023-07-23T14:37:00</v>
+      </c>
+      <c r="F1770" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1770" t="str">
+        <v>./mid_thumbs/123/IMG_7939.jpg</v>
+      </c>
+      <c r="H1770" t="str">
+        <v>./small_thumbs/123/IMG_7939.jpg</v>
+      </c>
+    </row>
+    <row r="1771">
+      <c r="A1771">
+        <v>1777</v>
+      </c>
+      <c r="B1771">
+        <v>123</v>
+      </c>
+      <c r="C1771" t="str">
+        <v>佐保川地蔵尊 地蔵盆</v>
+      </c>
+      <c r="D1771" t="str">
+        <v>./images/123/IMG_7940.jpg</v>
+      </c>
+      <c r="E1771" t="str">
+        <v>2023-07-23T14:37:03</v>
+      </c>
+      <c r="F1771" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1771" t="str">
+        <v>./mid_thumbs/123/IMG_7940.jpg</v>
+      </c>
+      <c r="H1771" t="str">
+        <v>./small_thumbs/123/IMG_7940.jpg</v>
+      </c>
+    </row>
+    <row r="1772">
+      <c r="A1772">
+        <v>1778</v>
+      </c>
+      <c r="B1772">
+        <v>45</v>
+      </c>
+      <c r="C1772" t="str">
+        <v>橋北地蔵尊 地蔵盆内部</v>
+      </c>
+      <c r="D1772" t="str">
+        <v>./images/45/IMG_7941.jpg</v>
+      </c>
+      <c r="E1772" t="str">
+        <v>2023-07-23T14:42:28</v>
+      </c>
+      <c r="F1772" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1772" t="str">
+        <v>./mid_thumbs/45/IMG_7941.jpg</v>
+      </c>
+      <c r="H1772" t="str">
+        <v>./small_thumbs/45/IMG_7941.jpg</v>
+      </c>
+    </row>
+    <row r="1773">
+      <c r="A1773">
+        <v>1779</v>
+      </c>
+      <c r="B1773">
+        <v>45</v>
+      </c>
+      <c r="C1773" t="str">
+        <v>橋北地蔵尊 地蔵盆</v>
+      </c>
+      <c r="D1773" t="str">
+        <v>./images/45/IMG_7942.jpg</v>
+      </c>
+      <c r="E1773" t="str">
+        <v>2023-07-23T14:43:09</v>
+      </c>
+      <c r="F1773" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1773" t="str">
+        <v>./mid_thumbs/45/IMG_7942.jpg</v>
+      </c>
+      <c r="H1773" t="str">
+        <v>./small_thumbs/45/IMG_7942.jpg</v>
+      </c>
+    </row>
+    <row r="1774">
+      <c r="A1774">
+        <v>1780</v>
+      </c>
+      <c r="B1774">
+        <v>857</v>
+      </c>
+      <c r="C1774" t="str">
+        <v>持宝院五輪塔、浮彫五輪塔</v>
+      </c>
+      <c r="D1774" t="str">
+        <v>./images/857/IMG_7932.jpg</v>
+      </c>
+      <c r="E1774" t="str">
+        <v>2023-07-23T13:47:57</v>
+      </c>
+      <c r="F1774" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1774" t="str">
+        <v>./mid_thumbs/857/IMG_7932.jpg</v>
+      </c>
+      <c r="H1774" t="str">
+        <v>./small_thumbs/857/IMG_7932.jpg</v>
+      </c>
+    </row>
+    <row r="1775">
+      <c r="A1775">
+        <v>1781</v>
+      </c>
+      <c r="B1775">
+        <v>858</v>
+      </c>
+      <c r="C1775" t="str">
+        <v>正倉院東方地蔵群</v>
+      </c>
+      <c r="D1775" t="str">
+        <v>./images/858/IMG_7933.jpg</v>
+      </c>
+      <c r="E1775" t="str">
+        <v>2023-07-23T13:50:33</v>
+      </c>
+      <c r="F1775" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1775" t="str">
+        <v>./mid_thumbs/858/IMG_7933.jpg</v>
+      </c>
+      <c r="H1775" t="str">
+        <v>./small_thumbs/858/IMG_7933.jpg</v>
+      </c>
+    </row>
+    <row r="1776">
+      <c r="A1776">
+        <v>1782</v>
+      </c>
+      <c r="B1776">
+        <v>58</v>
+      </c>
+      <c r="C1776" t="str">
+        <v>大門地蔵尊 地蔵盆</v>
+      </c>
+      <c r="D1776" t="str">
+        <v>./images/58/IMG_7929.jpg</v>
+      </c>
+      <c r="E1776" t="str">
+        <v>2023-07-23T13:02:03</v>
+      </c>
+      <c r="F1776" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1776" t="str">
+        <v>./mid_thumbs/58/IMG_7929.jpg</v>
+      </c>
+      <c r="H1776" t="str">
+        <v>./small_thumbs/58/IMG_7929.jpg</v>
+      </c>
+    </row>
+    <row r="1777">
+      <c r="A1777">
+        <v>1783</v>
+      </c>
+      <c r="B1777">
+        <v>82</v>
+      </c>
+      <c r="C1777" t="str">
+        <v>十福地蔵尊 地蔵盆</v>
+      </c>
+      <c r="D1777" t="str">
+        <v>./images/82/IMG_7954.jpg</v>
+      </c>
+      <c r="E1777" t="str">
+        <v>2023-07-23T16:21:37</v>
+      </c>
+      <c r="F1777" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1777" t="str">
+        <v>./mid_thumbs/82/IMG_7954.jpg</v>
+      </c>
+      <c r="H1777" t="str">
+        <v>./small_thumbs/82/IMG_7954.jpg</v>
+      </c>
+    </row>
+    <row r="1778">
+      <c r="A1778">
+        <v>1784</v>
+      </c>
+      <c r="B1778">
+        <v>82</v>
+      </c>
+      <c r="C1778" t="str">
+        <v>十福地蔵尊 地蔵盆供物</v>
+      </c>
+      <c r="D1778" t="str">
+        <v>./images/82/IMG_7955.jpg</v>
+      </c>
+      <c r="E1778" t="str">
+        <v>2023-07-23T16:21:45</v>
+      </c>
+      <c r="F1778" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1778" t="str">
+        <v>./mid_thumbs/82/IMG_7955.jpg</v>
+      </c>
+      <c r="H1778" t="str">
+        <v>./small_thumbs/82/IMG_7955.jpg</v>
+      </c>
+    </row>
+    <row r="1779">
+      <c r="A1779">
+        <v>1785</v>
+      </c>
+      <c r="B1779">
+        <v>12</v>
+      </c>
+      <c r="C1779" t="str">
+        <v>東向北地蔵尊 地蔵盆</v>
+      </c>
+      <c r="D1779" t="str">
+        <v>./images/12/IMG_7957.jpg</v>
+      </c>
+      <c r="E1779" t="str">
+        <v>2023-07-23T16:27:58</v>
+      </c>
+      <c r="F1779" t="str">
+        <v>Kohei Otsuka</v>
+      </c>
+      <c r="G1779" t="str">
+        <v>./mid_thumbs/12/IMG_7957.jpg</v>
+      </c>
+      <c r="H1779" t="str">
+        <v>./small_thumbs/12/IMG_7957.jpg</v>
+      </c>
+    </row>
+    <row r="1780">
+      <c r="A1780">
+        <v>1786</v>
+      </c>
+      <c r="B1780">
+        <v>859</v>
+      </c>
+      <c r="C1780" t="str">
+        <v>西大寺赤田町地蔵堂１</v>
+      </c>
+      <c r="D1780" t="str">
+        <v>./images/859/344300461_3415341435347227_6027728242804109744_n.jpg</v>
+      </c>
+      <c r="E1780" t="str">
+        <v>2023-05-10T01:36:14</v>
+      </c>
+      <c r="F1780" t="str">
+        <v>Takeo Hidaka</v>
+      </c>
+      <c r="G1780" t="str">
+        <v>./mid_thumbs/859/344300461_3415341435347227_6027728242804109744_n.jpg</v>
+      </c>
+      <c r="H1780" t="str">
+        <v>./small_thumbs/859/344300461_3415341435347227_6027728242804109744_n.jpg</v>
+      </c>
+    </row>
+    <row r="1781">
+      <c r="A1781">
+        <v>1787</v>
+      </c>
+      <c r="B1781">
+        <v>859</v>
+      </c>
+      <c r="C1781" t="str">
+        <v>西大寺赤田町地蔵堂１</v>
+      </c>
+      <c r="D1781" t="str">
+        <v>./images/859/345871364_622424796433445_2780874164980509545_n.jpg</v>
+      </c>
+      <c r="E1781" t="str">
+        <v>2023-05-10T01:36:14</v>
+      </c>
+      <c r="F1781" t="str">
+        <v>Takeo Hidaka</v>
+      </c>
+      <c r="G1781" t="str">
+        <v>./mid_thumbs/859/345871364_622424796433445_2780874164980509545_n.jpg</v>
+      </c>
+      <c r="H1781" t="str">
+        <v>./small_thumbs/859/345871364_622424796433445_2780874164980509545_n.jpg</v>
+      </c>
+    </row>
+    <row r="1782">
+      <c r="A1782">
+        <v>1788</v>
+      </c>
+      <c r="B1782">
+        <v>860</v>
+      </c>
+      <c r="C1782" t="str">
+        <v>西大寺赤田町地蔵堂２</v>
+      </c>
+      <c r="D1782" t="str">
+        <v>./images/860/345993944_255222507041078_2092380315280962758_n.jpg</v>
+      </c>
+      <c r="E1782" t="str">
+        <v>2023-05-10T01:39:16</v>
+      </c>
+      <c r="F1782" t="str">
+        <v>Takeo Hidaka</v>
+      </c>
+      <c r="G1782" t="str">
+        <v>./mid_thumbs/860/345993944_255222507041078_2092380315280962758_n.jpg</v>
+      </c>
+      <c r="H1782" t="str">
+        <v>./small_thumbs/860/345993944_255222507041078_2092380315280962758_n.jpg</v>
+      </c>
+    </row>
+    <row r="1783">
+      <c r="A1783">
+        <v>1789</v>
+      </c>
+      <c r="B1783">
+        <v>860</v>
+      </c>
+      <c r="C1783" t="str">
+        <v>西大寺赤田町地蔵堂２</v>
+      </c>
+      <c r="D1783" t="str">
+        <v>./images/860/346106944_3484881208418093_669085364674185231_n.jpg</v>
+      </c>
+      <c r="E1783" t="str">
+        <v>2023-05-10T01:39:16</v>
+      </c>
+      <c r="F1783" t="str">
+        <v>Takeo Hidaka</v>
+      </c>
+      <c r="G1783" t="str">
+        <v>./mid_thumbs/860/346106944_3484881208418093_669085364674185231_n.jpg</v>
+      </c>
+      <c r="H1783" t="str">
+        <v>./small_thumbs/860/346106944_3484881208418093_669085364674185231_n.jpg</v>
+      </c>
+    </row>
+    <row r="1784">
+      <c r="A1784">
+        <v>1790</v>
+      </c>
+      <c r="B1784">
+        <v>10</v>
+      </c>
+      <c r="C1784" t="str">
+        <v>地蔵堂</v>
+      </c>
+      <c r="D1784" t="str">
+        <v>./images/10/336521203_760938945294855_8695039677405354475_n.jpg</v>
+      </c>
+      <c r="E1784" t="str">
+        <v>2023-03-16T01:42:53</v>
+      </c>
+      <c r="F1784" t="str">
+        <v>Takeo Hidaka</v>
+      </c>
+      <c r="G1784" t="str">
+        <v>./mid_thumbs/10/336521203_760938945294855_8695039677405354475_n.jpg</v>
+      </c>
+      <c r="H1784" t="str">
+        <v>./small_thumbs/10/336521203_760938945294855_8695039677405354475_n.jpg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1744"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1784"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>